<commit_message>
Atualizações referentes a documentação e login
</commit_message>
<xml_diff>
--- a/Documentação/em-andamento/TI_Product_Backlog_StrongBerry.xlsx
+++ b/Documentação/em-andamento/TI_Product_Backlog_StrongBerry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberta\Desktop\workspace\Bandtec\Projeto Sprint2\StrongBerry\Documentação\em-andamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BDAE0B-CE87-4AB0-AD6F-59066CC3B1B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C925F917-3718-43ED-B132-FD30E4462F39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2910" yWindow="960" windowWidth="15375" windowHeight="9705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1025,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6">
         <v>13</v>
@@ -1067,7 +1067,7 @@
         <v>43</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D16" s="6">
         <v>21</v>

</xml_diff>

<commit_message>
Adicionando pasta de apresentação
</commit_message>
<xml_diff>
--- a/Documentação/em-andamento/TI_Product_Backlog_StrongBerry.xlsx
+++ b/Documentação/em-andamento/TI_Product_Backlog_StrongBerry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SETH\Desktop\GitHub SB Lucas\StrongBerry\Documentação\em-andamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34ECC28-BE83-443E-BA09-4F288F158E59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71848F9C-2BBD-40A9-BB62-DB408032D200}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,7 +645,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.6640625" defaultRowHeight="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -908,7 +908,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F11" s="15">
         <v>44277</v>
@@ -929,7 +929,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="6">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F12" s="15">
         <v>44279</v>
@@ -951,7 +951,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="6">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F13" s="15">
         <v>44281</v>
@@ -972,7 +972,7 @@
         <v>13</v>
       </c>
       <c r="E14" s="6">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F14" s="15">
         <v>44286</v>
@@ -993,7 +993,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="6">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F15" s="15">
         <v>44287</v>
@@ -1014,7 +1014,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="6">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F16" s="15">
         <v>44293</v>
@@ -1035,7 +1035,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="6">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F17" s="15">
         <v>44300</v>
@@ -1056,7 +1056,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="6">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F18" s="15">
         <v>44305</v>

</xml_diff>